<commit_message>
completed merge road. now add change lanes
</commit_message>
<xml_diff>
--- a/Resource/2017_MCM_Problem_C_Data.xlsx
+++ b/Resource/2017_MCM_Problem_C_Data.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jtomicek\Desktop\2017 MCM Problems\Final\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CodingPlace\projects\secret_project\Resource\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="985" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="985"/>
   </bookViews>
   <sheets>
     <sheet name="parsed mile posts" sheetId="2" r:id="rId1"/>
@@ -163,7 +163,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -177,6 +177,12 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="2">
@@ -244,7 +250,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -524,8 +530,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I225"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I144" sqref="I144"/>
+    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
+      <selection activeCell="K132" sqref="K132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5786,8 +5792,9 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -5799,7 +5806,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
@@ -5871,6 +5878,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>